<commit_message>
Export, und E-Mail Teil aktualisiert
</commit_message>
<xml_diff>
--- a/UPL_Performer/Data/Config.xlsx
+++ b/UPL_Performer/Data/Config.xlsx
@@ -5,24 +5,37 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timotheus.vrettos\develop\develop_RPA\Untergrundplan\UPL_Performer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timotheus.vrettos\develop\develop_RPA\uipath-rpa_upl\UPL_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67489E42-9EBE-4482-AA73-F0289F3B9338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A10554-5A55-4C6A-B90C-CD2DBD6D3E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23400" yWindow="-1035" windowWidth="24465" windowHeight="16095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-41295" yWindow="-3450" windowWidth="27120" windowHeight="11970" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="77">
   <si>
     <t>Name</t>
   </si>
@@ -225,9 +238,6 @@
     <t>Utility path for saving temporary files. If left empty or not rooted a default folder is set . Will be deleted at end.</t>
   </si>
   <si>
-    <t>rpa001_LoB_Bescheide_SendEmails</t>
-  </si>
-  <si>
     <t>EmailSmtpServer</t>
   </si>
   <si>
@@ -250,6 +260,15 @@
   </si>
   <si>
     <t>Working_Folder</t>
+  </si>
+  <si>
+    <t>rpa009_Groupmailbox</t>
+  </si>
+  <si>
+    <t>rpa009_StatusEmailReceiver</t>
+  </si>
+  <si>
+    <t>rpa009_UPL_Performer</t>
   </si>
 </sst>
 </file>
@@ -629,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -680,7 +699,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -702,8 +721,8 @@
       <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>66</v>
+      <c r="B5" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -712,18 +731,18 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1727,8 +1746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B30" sqref="A30:B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2005,28 +2024,21 @@
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B29" s="5">
         <v>587</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A30" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
@@ -2998,6 +3010,7 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3005,8 +3018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3054,16 +3067,28 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
+      <c r="A2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
+      <c r="A3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" s="5"/>
-      <c r="B4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="6"/>

</xml_diff>